<commit_message>
update template with new command
</commit_message>
<xml_diff>
--- a/templates/templates.xlsx
+++ b/templates/templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d_ils\Desktop\Bubbless\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33694AB8-6793-4B05-9EDD-E5E9C75637A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938987AB-D74E-4BF5-AAF7-F3800B0D581D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3AA56522-8371-4575-AB8A-46A19F8442C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3AA56522-8371-4575-AB8A-46A19F8442C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
   <si>
     <t>COPYCOLUMN</t>
   </si>
@@ -273,6 +273,24 @@
   </si>
   <si>
     <t>Only command with a second tab. In this example, CM is the column to pull the data from, and "Name" is the title of the chart.</t>
+  </si>
+  <si>
+    <t>// Here is how we count across columns</t>
+  </si>
+  <si>
+    <t>COUNTIF</t>
+  </si>
+  <si>
+    <t>XX_COL, Value</t>
+  </si>
+  <si>
+    <t>XX_COL, Value2</t>
+  </si>
+  <si>
+    <t>Here, each record's value at column XX is compared to "Value" . If the values match, then a counter is incremented. You can have as many columns as you need</t>
+  </si>
+  <si>
+    <t>Only 2 columns shown here, but can have as many as neeeded.</t>
   </si>
 </sst>
 </file>
@@ -453,15 +471,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,37 +794,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA756B7-171C-431E-BDC4-27F50EFFD28B}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="131.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="144.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="16"/>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -818,7 +836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -830,13 +848,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -847,7 +865,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -858,13 +876,13 @@
       <c r="D8" s="7"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -876,13 +894,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
@@ -892,13 +910,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
@@ -910,13 +928,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
@@ -926,7 +944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
@@ -936,7 +954,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>4</v>
       </c>
@@ -946,14 +964,14 @@
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="14"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -963,7 +981,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
@@ -975,7 +993,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>25</v>
       </c>
@@ -985,7 +1003,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -995,7 +1013,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
@@ -1005,7 +1023,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -1015,7 +1033,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1025,7 +1043,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>25</v>
       </c>
@@ -1035,7 +1053,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>4</v>
       </c>
@@ -1045,8 +1063,8 @@
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>28</v>
       </c>
@@ -1056,7 +1074,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>29</v>
       </c>
@@ -1066,7 +1084,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>30</v>
       </c>
@@ -1076,7 +1094,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>31</v>
       </c>
@@ -1086,7 +1104,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>4</v>
       </c>
@@ -1096,8 +1114,8 @@
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>33</v>
       </c>
@@ -1105,7 +1123,7 @@
       <c r="C38" s="4"/>
       <c r="D38" s="12"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>34</v>
       </c>
@@ -1117,7 +1135,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>35</v>
       </c>
@@ -1127,7 +1145,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>4</v>
       </c>
@@ -1137,8 +1155,8 @@
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1146,7 +1164,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>47</v>
       </c>
@@ -1154,7 +1172,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>39</v>
       </c>
@@ -1164,7 +1182,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
@@ -1174,7 +1192,7 @@
       <c r="C46" s="3"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>41</v>
       </c>
@@ -1182,7 +1200,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>42</v>
       </c>
@@ -1192,7 +1210,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>23</v>
       </c>
@@ -1202,7 +1220,7 @@
       <c r="C49" s="3"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>49</v>
       </c>
@@ -1212,7 +1230,7 @@
       <c r="C50" s="3"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>41</v>
       </c>
@@ -1220,7 +1238,7 @@
       <c r="C51" s="3"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>45</v>
       </c>
@@ -1230,7 +1248,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>43</v>
       </c>
@@ -1240,7 +1258,7 @@
       <c r="C53" s="3"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>38</v>
       </c>
@@ -1250,7 +1268,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>41</v>
       </c>
@@ -1258,7 +1276,7 @@
       <c r="C55" s="3"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>35</v>
       </c>
@@ -1270,7 +1288,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>53</v>
       </c>
@@ -1282,7 +1300,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>4</v>
       </c>
@@ -1292,8 +1310,8 @@
       <c r="C58" s="9"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>0</v>
       </c>
@@ -1305,7 +1323,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>4</v>
       </c>
@@ -1315,20 +1333,20 @@
       <c r="C61" s="3"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="13" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="13"/>
-    </row>
-    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>59</v>
       </c>
@@ -1338,7 +1356,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>1</v>
       </c>
@@ -1346,7 +1364,7 @@
       <c r="C67" s="3"/>
       <c r="D67" s="5"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>3</v>
       </c>
@@ -1354,7 +1372,7 @@
       <c r="C68" s="3"/>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>60</v>
       </c>
@@ -1362,8 +1380,8 @@
       <c r="C69" s="9"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>62</v>
       </c>
@@ -1373,7 +1391,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>64</v>
       </c>
@@ -1381,7 +1399,7 @@
       <c r="C72" s="3"/>
       <c r="D72" s="5"/>
     </row>
-    <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>60</v>
       </c>
@@ -1389,8 +1407,8 @@
       <c r="C73" s="9"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>65</v>
       </c>
@@ -1402,7 +1420,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>70</v>
       </c>
@@ -1410,7 +1428,7 @@
       <c r="C76" s="3"/>
       <c r="D76" s="5"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>67</v>
       </c>
@@ -1420,7 +1438,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>68</v>
       </c>
@@ -1428,7 +1446,7 @@
       <c r="C78" s="3"/>
       <c r="D78" s="5"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>69</v>
       </c>
@@ -1436,7 +1454,7 @@
       <c r="C79" s="3"/>
       <c r="D79" s="5"/>
     </row>
-    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
         <v>71</v>
       </c>
@@ -1446,30 +1464,60 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="13" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-    </row>
-    <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="85" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="15" t="s">
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C85" s="16" t="s">
+      <c r="C85" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D85" s="17" t="s">
+      <c r="D85" s="15" t="s">
         <v>79</v>
       </c>
     </row>
+    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="8"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A89:C89"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A20:B20"/>

</xml_diff>